<commit_message>
Update comments for ports and baudrates.
</commit_message>
<xml_diff>
--- a/notas/powercurvasquad.xlsx
+++ b/notas/powercurvasquad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matro\Documents\AIUC\Scripts\RFLabTests\notas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A104DFCA-E429-4E70-8911-BE8BFE086E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190C959E-C6D5-4F10-AD9D-611BC8DC9FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="5" xr2:uid="{1B3B1B6B-8F0B-4D4E-8B6F-5AE4CB87CC58}"/>
   </bookViews>
@@ -33159,7 +33159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0AC145-901E-41FF-BD54-679511BE3629}">
   <dimension ref="B2:AB25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="104" zoomScaleNormal="265" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="104" zoomScaleNormal="265" workbookViewId="0">
       <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>

</xml_diff>